<commit_message>
Address inser was added
</commit_message>
<xml_diff>
--- a/fileHandler/addresses.xlsx
+++ b/fileHandler/addresses.xlsx
@@ -20,15 +20,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+  <si>
+    <t xml:space="preserve">4001 South 700 East</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1060 Dalton Ave S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1330 2100 S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1488 4800 S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">177 W Price Ave</t>
+  </si>
   <si>
     <t xml:space="preserve">195 W Oakland Ave</t>
   </si>
   <si>
-    <t xml:space="preserve">2530 S 500 E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">233 Canyon Rd</t>
+    <t xml:space="preserve">2010 W 500 S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2300 Parkway Blvd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2600 Taylorsville Blvd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2835 Main St</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 State St</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3060 Lester St</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3148 S 1100 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3365 S 900 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3575 W Valley Central Sta bus Loop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3595 Main St</t>
   </si>
   <si>
     <t xml:space="preserve">380 W 2880 S</t>
@@ -37,67 +76,25 @@
     <t xml:space="preserve">410 S State St</t>
   </si>
   <si>
-    <t xml:space="preserve">3060 Lester St</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1330 2100 S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">300 State St</t>
+    <t xml:space="preserve">4300 S 1300 E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4580 S 2300 E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5025 State St</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5100 South 2700 West</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5383 South 900 East #104</t>
   </si>
   <si>
     <t xml:space="preserve">600 E 900 South</t>
   </si>
   <si>
-    <t xml:space="preserve">2600 Taylorsville Blvd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3575 W Valley Central Station bus Loop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2010 W 500 S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4300 S 1300 E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4580 S 2300 E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3148 S 1100 W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1488 4800 S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">177 W Price Ave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3595 Main St</t>
-  </si>
-  <si>
     <t xml:space="preserve">6351 South 900 East</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5100 South 2700 West</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5025 State St</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5383 South 900 East #104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1060 Dalton Ave S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2835 Main St</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3365 S 900 W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2300 Parkway Blvd</t>
   </si>
 </sst>
 </file>
@@ -154,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -163,10 +160,17 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+      <left style="medium"/>
+      <right style="medium"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
   </borders>
@@ -195,13 +199,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -220,6 +224,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -232,57 +244,15 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1561680</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>162360</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Picture 2" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1561680" y="60840"/>
-          <a:ext cx="4608360" cy="415440"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ48"/>
+  <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -296,7 +266,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="39.79"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -358,12 +328,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" s="5" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" s="5" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -383,178 +353,110 @@
       <c r="AMI8" s="0"/>
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+    <row r="9" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+    <row r="10" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+    <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+    <row r="14" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+    <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+    <row r="16" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+    <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+    <row r="18" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+    <row r="19" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+    <row r="20" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+    <row r="21" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+    <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+    <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+    <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+    <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C1:H3"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -562,7 +464,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Distance was added to graph
</commit_message>
<xml_diff>
--- a/fileHandler/addresses.xlsx
+++ b/fileHandler/addresses.xlsx
@@ -20,81 +20,109 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">4001 South 700 East</t>
   </si>
   <si>
-    <t xml:space="preserve">1060 Dalton Ave S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1330 2100 S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1488 4800 S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">177 W Price Ave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">195 W Oakland Ave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2010 W 500 S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2300 Parkway Blvd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2600 Taylorsville Blvd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2835 Main St</t>
-  </si>
-  <si>
-    <t xml:space="preserve">300 State St</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3060 Lester St</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3148 S 1100 W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3365 S 900 W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3575 W Valley Central Sta bus Loop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3595 Main St</t>
-  </si>
-  <si>
-    <t xml:space="preserve">380 W 2880 S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">410 S State St</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4300 S 1300 E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4580 S 2300 E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5025 State St</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5100 South 2700 West</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5383 South 900 East #104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">600 E 900 South</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6351 South 900 East</t>
+    <t xml:space="preserve"> 1060 Dalton Ave S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1330 2100 S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1488 4800 S
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 177 W Price Ave
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 195 W Oakland Ave
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2010 W 500 S
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2300 Parkway Blvd
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 233 Canyon Rd
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2530 S 500 E
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2600 Taylorsville Blvd
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2835 Main St
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 300 State St</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3060 Lester St
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3148 S 1100 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3365 S 900 W
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3575 W Valley Central Station bus Loop
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3595 Main St
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 380 W 2880 S
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 410 S State St
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4300 S 1300 E
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4580 S 2300 E
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5025 State St
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5100 South 2700 West
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5383 S 900 East #104
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 600 E 900 South
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6351 South 900 East
+</t>
   </si>
 </sst>
 </file>
@@ -104,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -128,13 +156,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="16"/>
       <color rgb="FF000000"/>
@@ -151,26 +172,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
       <diagonal/>
     </border>
   </borders>
@@ -199,38 +206,34 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -249,21 +252,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ35"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="39.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="39.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="3.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="39.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="8.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -281,8 +286,8 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2"/>
@@ -296,7 +301,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -311,141 +316,126 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="4" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+    <row r="7" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" s="5" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+    <row r="8" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="0"/>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-      <c r="F8" s="0"/>
-      <c r="G8" s="0"/>
-      <c r="H8" s="0"/>
-      <c r="AMC8" s="0"/>
-      <c r="AMD8" s="0"/>
-      <c r="AME8" s="0"/>
-      <c r="AMF8" s="0"/>
-      <c r="AMG8" s="0"/>
-      <c r="AMH8" s="0"/>
-      <c r="AMI8" s="0"/>
-      <c r="AMJ8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+    <row r="10" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+    <row r="11" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+    <row r="13" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+    <row r="15" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+    <row r="16" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
-        <v>8</v>
+      <c r="A26" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="s">
-        <v>9</v>
+      <c r="A27" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
First truck was loaded
</commit_message>
<xml_diff>
--- a/fileHandler/addresses.xlsx
+++ b/fileHandler/addresses.xlsx
@@ -25,103 +25,103 @@
     <t xml:space="preserve">4001 South 700 East</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1060 Dalton Ave S</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1330 2100 S</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1488 4800 S
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 177 W Price Ave
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 195 W Oakland Ave
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2010 W 500 S
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2300 Parkway Blvd
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 233 Canyon Rd
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2530 S 500 E
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2600 Taylorsville Blvd
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2835 Main St
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 300 State St</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3060 Lester St
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3148 S 1100 W</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3365 S 900 W
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3575 W Valley Central Station bus Loop
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3595 Main St
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 380 W 2880 S
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 410 S State St
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4300 S 1300 E
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4580 S 2300 E
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5025 State St
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5100 South 2700 West
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5383 S 900 East #104
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 600 E 900 South
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6351 South 900 East
+    <t xml:space="preserve">1060 Dalton Ave S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1330 2100 S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1488 4800 S
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">177 W Price Ave
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">195 W Oakland Ave
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2010 W 500 S
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2300 Parkway Blvd
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">233 Canyon Rd
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2530 S 500 E
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2600 Taylorsville Blvd
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2835 Main St
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 State St</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3060 Lester St
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3148 S 1100 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3365 S 900 W
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3575 W Valley Central Station bus Loop
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3595 Main St
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">380 W 2880 S
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">410 S State St
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4300 S 1300 E
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4580 S 2300 E
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5025 State St
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5100 South 2700 West
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5383 S 900 East #104
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">600 E 900 South
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6351 South 900 East
 </t>
   </si>
 </sst>
@@ -255,10 +255,10 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="39.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.11"/>

</xml_diff>

<commit_message>
Get distance between first and next addresses
</commit_message>
<xml_diff>
--- a/fileHandler/addresses.xlsx
+++ b/fileHandler/addresses.xlsx
@@ -31,98 +31,76 @@
     <t xml:space="preserve">1330 2100 S</t>
   </si>
   <si>
-    <t xml:space="preserve">1488 4800 S
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">177 W Price Ave
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">195 W Oakland Ave
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2010 W 500 S
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2300 Parkway Blvd
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">233 Canyon Rd
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2530 S 500 E
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2600 Taylorsville Blvd
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2835 Main St
-</t>
+    <t xml:space="preserve">1488 4800 S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">177 W Price Ave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">195 W Oakland Ave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2010 W 500 S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2300 Parkway Blvd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">233 Canyon Rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2530 S 500 E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2600 Taylorsville Blvd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2835 Main St</t>
   </si>
   <si>
     <t xml:space="preserve">300 State St</t>
   </si>
   <si>
-    <t xml:space="preserve">3060 Lester St
-</t>
+    <t xml:space="preserve">3060 Lester St</t>
   </si>
   <si>
     <t xml:space="preserve">3148 S 1100 W</t>
   </si>
   <si>
-    <t xml:space="preserve">3365 S 900 W
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3575 W Valley Central Station bus Loop
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3595 Main St
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">380 W 2880 S
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">410 S State St
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4300 S 1300 E
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4580 S 2300 E
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5025 State St
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5100 South 2700 West
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5383 S 900 East #104
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">600 E 900 South
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6351 South 900 East
-</t>
+    <t xml:space="preserve">3365 S 900 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3575 W Valley Central Station bus Loop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3595 Main St</t>
+  </si>
+  <si>
+    <t xml:space="preserve">380 W 2880 S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">410 S State St</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4300 S 1300 E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4580 S 2300 E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5025 State St</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5100 South 2700 West</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5383 S 900 East #104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">600 E 900 South</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6351 South 900 East</t>
   </si>
 </sst>
 </file>
@@ -255,7 +233,7 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -378,7 +356,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Both trucks came back
</commit_message>
<xml_diff>
--- a/fileHandler/addresses.xlsx
+++ b/fileHandler/addresses.xlsx
@@ -94,7 +94,7 @@
     <t xml:space="preserve">5100 South 2700 West</t>
   </si>
   <si>
-    <t xml:space="preserve">5383 S 900 East #104</t>
+    <t xml:space="preserve">5383 South 900 East #104</t>
   </si>
   <si>
     <t xml:space="preserve">600 E 900 South</t>
@@ -232,8 +232,8 @@
   </sheetPr>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>